<commit_message>
Dane o aktywach finansowych
</commit_message>
<xml_diff>
--- a/Dane/CEX.xlsx
+++ b/Dane/CEX.xlsx
@@ -486,25 +486,25 @@
         <v>30682</v>
       </c>
       <c r="B2" t="n">
-        <v>27100.32901861247</v>
+        <v>27585.55900144784</v>
       </c>
       <c r="C2" t="n">
-        <v>45417.30583020655</v>
+        <v>46230.50033102927</v>
       </c>
       <c r="D2" t="n">
-        <v>57720.17824365318</v>
+        <v>58753.65503573159</v>
       </c>
       <c r="E2" t="n">
-        <v>59295.76076055646</v>
+        <v>60357.44827572616</v>
       </c>
       <c r="F2" t="n">
-        <v>47700.15847940661</v>
+        <v>48554.2273382869</v>
       </c>
       <c r="G2" t="n">
-        <v>33047.58640402355</v>
+        <v>33639.30172130118</v>
       </c>
       <c r="H2" t="n">
-        <v>23240.09925868209</v>
+        <v>23656.21202825921</v>
       </c>
     </row>
     <row r="3">
@@ -512,25 +512,25 @@
         <v>31048</v>
       </c>
       <c r="B3" t="n">
-        <v>27343.8938962482</v>
+        <v>27833.48489556097</v>
       </c>
       <c r="C3" t="n">
-        <v>45718.845170165</v>
+        <v>46537.43871720046</v>
       </c>
       <c r="D3" t="n">
-        <v>58555.66769922608</v>
+        <v>59604.10388659112</v>
       </c>
       <c r="E3" t="n">
-        <v>60031.22283092645</v>
+        <v>61106.07875624853</v>
       </c>
       <c r="F3" t="n">
-        <v>47891.9942577223</v>
+        <v>48749.49792624477</v>
       </c>
       <c r="G3" t="n">
-        <v>33919.85689486239</v>
+        <v>34527.19016995178</v>
       </c>
       <c r="H3" t="n">
-        <v>23658.83502775388</v>
+        <v>24082.44523951698</v>
       </c>
     </row>
     <row r="4">
@@ -538,25 +538,25 @@
         <v>31413</v>
       </c>
       <c r="B4" t="n">
-        <v>27625.72088559936</v>
+        <v>28120.35798251159</v>
       </c>
       <c r="C4" t="n">
-        <v>45995.44418848711</v>
+        <v>46818.99022657244</v>
       </c>
       <c r="D4" t="n">
-        <v>59328.47051638073</v>
+        <v>60390.74369802895</v>
       </c>
       <c r="E4" t="n">
-        <v>60602.33958557488</v>
+        <v>61687.42132671152</v>
       </c>
       <c r="F4" t="n">
-        <v>48051.98998465517</v>
+        <v>48912.35836835435</v>
       </c>
       <c r="G4" t="n">
-        <v>34663.03127912778</v>
+        <v>35283.67105294909</v>
       </c>
       <c r="H4" t="n">
-        <v>23973.47224109043</v>
+        <v>24402.7160158085</v>
       </c>
     </row>
     <row r="5">
@@ -564,25 +564,25 @@
         <v>31778</v>
       </c>
       <c r="B5" t="n">
-        <v>27939.87737197545</v>
+        <v>28440.1394244515</v>
       </c>
       <c r="C5" t="n">
-        <v>46255.10620060921</v>
+        <v>47083.30147352849</v>
       </c>
       <c r="D5" t="n">
-        <v>59909.33973982602</v>
+        <v>60982.0133547357</v>
       </c>
       <c r="E5" t="n">
-        <v>60967.94086194292</v>
+        <v>62059.56867493501</v>
       </c>
       <c r="F5" t="n">
-        <v>48280.48998502469</v>
+        <v>49144.94964935679</v>
       </c>
       <c r="G5" t="n">
-        <v>35337.27410058252</v>
+        <v>35969.98615708572</v>
       </c>
       <c r="H5" t="n">
-        <v>24373.35430765165</v>
+        <v>24809.75794999196</v>
       </c>
     </row>
     <row r="6">
@@ -590,25 +590,25 @@
         <v>32143</v>
       </c>
       <c r="B6" t="n">
-        <v>28222.54892097718</v>
+        <v>28727.87219284945</v>
       </c>
       <c r="C6" t="n">
-        <v>46531.8552403543</v>
+        <v>47365.0056904493</v>
       </c>
       <c r="D6" t="n">
-        <v>60307.84045966132</v>
+        <v>61387.64920925194</v>
       </c>
       <c r="E6" t="n">
-        <v>61332.95485575496</v>
+        <v>62431.11822533877</v>
       </c>
       <c r="F6" t="n">
-        <v>48646.62018387501</v>
+        <v>49517.63539039208</v>
       </c>
       <c r="G6" t="n">
-        <v>35857.66827481519</v>
+        <v>36499.6979619663</v>
       </c>
       <c r="H6" t="n">
-        <v>24986.2901179968</v>
+        <v>25433.66834417072</v>
       </c>
     </row>
     <row r="7">
@@ -616,25 +616,25 @@
         <v>32509</v>
       </c>
       <c r="B7" t="n">
-        <v>28259.20711410587</v>
+        <v>28765.18674902109</v>
       </c>
       <c r="C7" t="n">
-        <v>46737.62404614226</v>
+        <v>47574.45877601231</v>
       </c>
       <c r="D7" t="n">
-        <v>60425.87627407055</v>
+        <v>61507.79844878455</v>
       </c>
       <c r="E7" t="n">
-        <v>61696.13121039236</v>
+        <v>62800.79723373384</v>
       </c>
       <c r="F7" t="n">
-        <v>49238.90876613978</v>
+        <v>50120.52886894477</v>
       </c>
       <c r="G7" t="n">
-        <v>36170.53405439614</v>
+        <v>36818.16558707281</v>
       </c>
       <c r="H7" t="n">
-        <v>25719.81802528049</v>
+        <v>26180.33003051723</v>
       </c>
     </row>
     <row r="8">
@@ -642,25 +642,25 @@
         <v>32874</v>
       </c>
       <c r="B8" t="n">
-        <v>28076.5559348347</v>
+        <v>28579.26520987642</v>
       </c>
       <c r="C8" t="n">
-        <v>46833.68567799003</v>
+        <v>47672.24038638664</v>
       </c>
       <c r="D8" t="n">
-        <v>60139.86974979974</v>
+        <v>61216.67099255863</v>
       </c>
       <c r="E8" t="n">
-        <v>61898.27034442579</v>
+        <v>63006.55565845839</v>
       </c>
       <c r="F8" t="n">
-        <v>49849.54537548058</v>
+        <v>50742.09889504485</v>
       </c>
       <c r="G8" t="n">
-        <v>36338.94105057482</v>
+        <v>36989.58790176683</v>
       </c>
       <c r="H8" t="n">
-        <v>26345.74385183715</v>
+        <v>26817.46302647276</v>
       </c>
     </row>
     <row r="9">
@@ -668,25 +668,25 @@
         <v>33239</v>
       </c>
       <c r="B9" t="n">
-        <v>27820.85429002583</v>
+        <v>28318.98524040454</v>
       </c>
       <c r="C9" t="n">
-        <v>46771.94219740704</v>
+        <v>47609.39139199234</v>
       </c>
       <c r="D9" t="n">
-        <v>59619.28798692698</v>
+        <v>60686.76824027306</v>
       </c>
       <c r="E9" t="n">
-        <v>62002.26434216783</v>
+        <v>63112.41166332595</v>
       </c>
       <c r="F9" t="n">
-        <v>50394.48213754586</v>
+        <v>51296.79272151761</v>
       </c>
       <c r="G9" t="n">
-        <v>36562.28148388504</v>
+        <v>37216.92723392993</v>
       </c>
       <c r="H9" t="n">
-        <v>26955.60923533765</v>
+        <v>27438.24801797381</v>
       </c>
     </row>
     <row r="10">
@@ -694,25 +694,25 @@
         <v>33604</v>
       </c>
       <c r="B10" t="n">
-        <v>27601.67989130094</v>
+        <v>28095.88653545968</v>
       </c>
       <c r="C10" t="n">
-        <v>46597.09521157374</v>
+        <v>47431.41377996354</v>
       </c>
       <c r="D10" t="n">
-        <v>59013.30978666624</v>
+        <v>60069.94003182562</v>
       </c>
       <c r="E10" t="n">
-        <v>62153.93010655557</v>
+        <v>63266.792995344</v>
       </c>
       <c r="F10" t="n">
-        <v>50703.31500371301</v>
+        <v>51611.1552241052</v>
       </c>
       <c r="G10" t="n">
-        <v>36864.6185268327</v>
+        <v>37524.67760592084</v>
       </c>
       <c r="H10" t="n">
-        <v>27600.94035519694</v>
+        <v>28095.13375800016</v>
       </c>
     </row>
     <row r="11">
@@ -720,25 +720,25 @@
         <v>33970</v>
       </c>
       <c r="B11" t="n">
-        <v>27444.28934982923</v>
+        <v>27935.67792452151</v>
       </c>
       <c r="C11" t="n">
-        <v>46509.14593341768</v>
+        <v>47341.88977455212</v>
       </c>
       <c r="D11" t="n">
-        <v>58439.06244709114</v>
+        <v>59485.41082347586</v>
       </c>
       <c r="E11" t="n">
-        <v>62533.1672971669</v>
+        <v>63652.82040814641</v>
       </c>
       <c r="F11" t="n">
-        <v>50874.72339007859</v>
+        <v>51785.63266872131</v>
       </c>
       <c r="G11" t="n">
-        <v>37310.37690086897</v>
+        <v>37978.41726048096</v>
       </c>
       <c r="H11" t="n">
-        <v>28130.12245385691</v>
+        <v>28633.7908346382</v>
       </c>
     </row>
     <row r="12">
@@ -746,25 +746,25 @@
         <v>34335</v>
       </c>
       <c r="B12" t="n">
-        <v>27360.94609783565</v>
+        <v>27850.84241593184</v>
       </c>
       <c r="C12" t="n">
-        <v>46792.28961552368</v>
+        <v>47630.10312957286</v>
       </c>
       <c r="D12" t="n">
-        <v>58057.00362663296</v>
+        <v>59096.51125969081</v>
       </c>
       <c r="E12" t="n">
-        <v>62916.69280225705</v>
+        <v>64043.21291747566</v>
       </c>
       <c r="F12" t="n">
-        <v>50987.38394330539</v>
+        <v>51900.31040329915</v>
       </c>
       <c r="G12" t="n">
-        <v>37901.03902453736</v>
+        <v>38579.65515878052</v>
       </c>
       <c r="H12" t="n">
-        <v>28507.21239102461</v>
+        <v>29017.63254753576</v>
       </c>
     </row>
     <row r="13">
@@ -772,25 +772,25 @@
         <v>34700</v>
       </c>
       <c r="B13" t="n">
-        <v>27326.97652315638</v>
+        <v>27816.26461778318</v>
       </c>
       <c r="C13" t="n">
-        <v>47414.99503350398</v>
+        <v>48263.95805570389</v>
       </c>
       <c r="D13" t="n">
-        <v>58003.45003174619</v>
+        <v>59041.99879047045</v>
       </c>
       <c r="E13" t="n">
-        <v>63295.13688414163</v>
+        <v>64428.43302098078</v>
       </c>
       <c r="F13" t="n">
-        <v>51199.63907336416</v>
+        <v>52116.36595043198</v>
       </c>
       <c r="G13" t="n">
-        <v>38576.05466455982</v>
+        <v>39266.75691876117</v>
       </c>
       <c r="H13" t="n">
-        <v>28770.72680430463</v>
+        <v>29285.86517269223</v>
       </c>
     </row>
     <row r="14">
@@ -798,25 +798,25 @@
         <v>35065</v>
       </c>
       <c r="B14" t="n">
-        <v>27433.40333082388</v>
+        <v>27924.59699191165</v>
       </c>
       <c r="C14" t="n">
-        <v>48295.81908069666</v>
+        <v>49160.55321169037</v>
       </c>
       <c r="D14" t="n">
-        <v>58295.18938379692</v>
+        <v>59338.96172045969</v>
       </c>
       <c r="E14" t="n">
-        <v>63700.63625680143</v>
+        <v>64841.19283883668</v>
       </c>
       <c r="F14" t="n">
-        <v>51735.21524611041</v>
+        <v>52661.53158672046</v>
       </c>
       <c r="G14" t="n">
-        <v>39323.92755562317</v>
+        <v>40028.02043507651</v>
       </c>
       <c r="H14" t="n">
-        <v>29106.85819939279</v>
+        <v>29628.0149829427</v>
       </c>
     </row>
     <row r="15">
@@ -824,25 +824,25 @@
         <v>35431</v>
       </c>
       <c r="B15" t="n">
-        <v>27806.3237977336</v>
+        <v>28304.19458040293</v>
       </c>
       <c r="C15" t="n">
-        <v>49290.33445418716</v>
+        <v>50172.875331264</v>
       </c>
       <c r="D15" t="n">
-        <v>58850.40074349465</v>
+        <v>59904.1141107019</v>
       </c>
       <c r="E15" t="n">
-        <v>64120.01458451613</v>
+        <v>65268.08011371663</v>
       </c>
       <c r="F15" t="n">
-        <v>52416.90048042664</v>
+        <v>53355.42235973399</v>
       </c>
       <c r="G15" t="n">
-        <v>39995.58801989866</v>
+        <v>40711.70694506259</v>
       </c>
       <c r="H15" t="n">
-        <v>29539.30575168374</v>
+        <v>30068.20548618569</v>
       </c>
     </row>
     <row r="16">
@@ -850,25 +850,25 @@
         <v>35796</v>
       </c>
       <c r="B16" t="n">
-        <v>28506.78473113119</v>
+        <v>29017.19723041427</v>
       </c>
       <c r="C16" t="n">
-        <v>50267.6265615446</v>
+        <v>51167.66580301944</v>
       </c>
       <c r="D16" t="n">
-        <v>59638.16637950928</v>
+        <v>60705.98464949397</v>
       </c>
       <c r="E16" t="n">
-        <v>64384.45615627223</v>
+        <v>65537.25649807356</v>
       </c>
       <c r="F16" t="n">
-        <v>53267.30938772083</v>
+        <v>54221.05779432267</v>
       </c>
       <c r="G16" t="n">
-        <v>40654.41853658425</v>
+        <v>41382.33378791394</v>
       </c>
       <c r="H16" t="n">
-        <v>30035.94355020801</v>
+        <v>30573.73555868528</v>
       </c>
     </row>
     <row r="17">
@@ -876,25 +876,25 @@
         <v>36161</v>
       </c>
       <c r="B17" t="n">
-        <v>29403.40963852509</v>
+        <v>29929.87616018286</v>
       </c>
       <c r="C17" t="n">
-        <v>51258.05448060479</v>
+        <v>52175.82728250376</v>
       </c>
       <c r="D17" t="n">
-        <v>60534.6002218842</v>
+        <v>61618.46909323441</v>
       </c>
       <c r="E17" t="n">
-        <v>64501.95479635284</v>
+        <v>65656.85894519911</v>
       </c>
       <c r="F17" t="n">
-        <v>54217.55020290917</v>
+        <v>55188.31262192879</v>
       </c>
       <c r="G17" t="n">
-        <v>41382.43672564317</v>
+        <v>42123.38710481712</v>
       </c>
       <c r="H17" t="n">
-        <v>30514.0523423179</v>
+        <v>31060.40486387349</v>
       </c>
     </row>
     <row r="18">
@@ -902,25 +902,25 @@
         <v>36526</v>
       </c>
       <c r="B18" t="n">
-        <v>30216.74261375064</v>
+        <v>30757.77182006581</v>
       </c>
       <c r="C18" t="n">
-        <v>52182.70605916309</v>
+        <v>53117.0346995275</v>
       </c>
       <c r="D18" t="n">
-        <v>61488.0341963397</v>
+        <v>62588.97425345836</v>
       </c>
       <c r="E18" t="n">
-        <v>64556.64469972534</v>
+        <v>65712.52806844948</v>
       </c>
       <c r="F18" t="n">
-        <v>55189.19578423923</v>
+        <v>56177.35546690203</v>
       </c>
       <c r="G18" t="n">
-        <v>42105.6456257308</v>
+        <v>42859.54502267989</v>
       </c>
       <c r="H18" t="n">
-        <v>30868.35001730871</v>
+        <v>31421.04622032432</v>
       </c>
     </row>
     <row r="19">
@@ -928,25 +928,25 @@
         <v>36892</v>
       </c>
       <c r="B19" t="n">
-        <v>30820.99334594914</v>
+        <v>31372.84163022501</v>
       </c>
       <c r="C19" t="n">
-        <v>52889.11638860084</v>
+        <v>53836.09326920588</v>
       </c>
       <c r="D19" t="n">
-        <v>62384.34314540044</v>
+        <v>63501.33156767619</v>
       </c>
       <c r="E19" t="n">
-        <v>64777.53494281383</v>
+        <v>65937.37333986211</v>
       </c>
       <c r="F19" t="n">
-        <v>56291.80448694943</v>
+        <v>57299.70632113834</v>
       </c>
       <c r="G19" t="n">
-        <v>42845.68753626301</v>
+        <v>43612.83734516452</v>
       </c>
       <c r="H19" t="n">
-        <v>31254.6341354758</v>
+        <v>31814.2467355543</v>
       </c>
     </row>
     <row r="20">
@@ -954,25 +954,25 @@
         <v>37257</v>
       </c>
       <c r="B20" t="n">
-        <v>31211.8072953947</v>
+        <v>31770.65308312707</v>
       </c>
       <c r="C20" t="n">
-        <v>53440.09801610061</v>
+        <v>54396.9401941148</v>
       </c>
       <c r="D20" t="n">
-        <v>63200.40787423147</v>
+        <v>64332.00789307091</v>
       </c>
       <c r="E20" t="n">
-        <v>65221.06543330044</v>
+        <v>66388.84522073313</v>
       </c>
       <c r="F20" t="n">
-        <v>57459.9714223789</v>
+        <v>58488.7892248441</v>
       </c>
       <c r="G20" t="n">
-        <v>43662.58801776014</v>
+        <v>44444.36438733333</v>
       </c>
       <c r="H20" t="n">
-        <v>31713.42952025936</v>
+        <v>32281.25682786161</v>
       </c>
     </row>
     <row r="21">
@@ -980,25 +980,25 @@
         <v>37622</v>
       </c>
       <c r="B21" t="n">
-        <v>31521.48699434815</v>
+        <v>32085.87758099802</v>
       </c>
       <c r="C21" t="n">
-        <v>53930.16588655756</v>
+        <v>54895.78270432636</v>
       </c>
       <c r="D21" t="n">
-        <v>64026.20322286293</v>
+        <v>65172.58906450796</v>
       </c>
       <c r="E21" t="n">
-        <v>65894.77162546522</v>
+        <v>67074.61408725999</v>
       </c>
       <c r="F21" t="n">
-        <v>58533.63328511273</v>
+        <v>59581.67494743838</v>
       </c>
       <c r="G21" t="n">
-        <v>44657.55544127778</v>
+        <v>45457.14665086652</v>
       </c>
       <c r="H21" t="n">
-        <v>32256.28886236092</v>
+        <v>32833.83603827428</v>
       </c>
     </row>
     <row r="22">
@@ -1006,25 +1006,25 @@
         <v>37987</v>
       </c>
       <c r="B22" t="n">
-        <v>32030.92662222056</v>
+        <v>32604.43869893488</v>
       </c>
       <c r="C22" t="n">
-        <v>54450.00933441606</v>
+        <v>55424.93392210561</v>
       </c>
       <c r="D22" t="n">
-        <v>65087.51887889869</v>
+        <v>66252.90752221478</v>
       </c>
       <c r="E22" t="n">
-        <v>66698.93865558253</v>
+        <v>67893.17968626379</v>
       </c>
       <c r="F22" t="n">
-        <v>59544.81745233371</v>
+        <v>60610.96431462823</v>
       </c>
       <c r="G22" t="n">
-        <v>45778.11569008718</v>
+        <v>46597.77047270192</v>
       </c>
       <c r="H22" t="n">
-        <v>32854.19861057224</v>
+        <v>33442.45132945751</v>
       </c>
     </row>
     <row r="23">
@@ -1032,25 +1032,25 @@
         <v>38353</v>
       </c>
       <c r="B23" t="n">
-        <v>32619.18736016208</v>
+        <v>33203.23221482083</v>
       </c>
       <c r="C23" t="n">
-        <v>54878.55181643882</v>
+        <v>55861.14943500017</v>
       </c>
       <c r="D23" t="n">
-        <v>66157.79573936954</v>
+        <v>67342.34763425634</v>
       </c>
       <c r="E23" t="n">
-        <v>67392.63364478406</v>
+        <v>68599.29524819963</v>
       </c>
       <c r="F23" t="n">
-        <v>60337.04483243186</v>
+        <v>61417.3764847997</v>
       </c>
       <c r="G23" t="n">
-        <v>46799.35461968444</v>
+        <v>47637.29463226591</v>
       </c>
       <c r="H23" t="n">
-        <v>33514.14608721247</v>
+        <v>34114.21513137338</v>
       </c>
     </row>
     <row r="24">
@@ -1058,25 +1058,25 @@
         <v>38718</v>
       </c>
       <c r="B24" t="n">
-        <v>32989.06630538854</v>
+        <v>33579.73382334111</v>
       </c>
       <c r="C24" t="n">
-        <v>55018.02305293289</v>
+        <v>56003.11789673618</v>
       </c>
       <c r="D24" t="n">
-        <v>66771.77180358404</v>
+        <v>67967.31690799592</v>
       </c>
       <c r="E24" t="n">
-        <v>67729.69045338577</v>
+        <v>68942.38704144454</v>
       </c>
       <c r="F24" t="n">
-        <v>60791.39455999131</v>
+        <v>61879.86132062114</v>
       </c>
       <c r="G24" t="n">
-        <v>47542.13667228798</v>
+        <v>48393.37615892335</v>
       </c>
       <c r="H24" t="n">
-        <v>34197.83500540497</v>
+        <v>34810.14546411882</v>
       </c>
     </row>
     <row r="25">
@@ -1084,25 +1084,25 @@
         <v>39083</v>
       </c>
       <c r="B25" t="n">
-        <v>33060.6272344586</v>
+        <v>33652.57604712757</v>
       </c>
       <c r="C25" t="n">
-        <v>54732.55273544707</v>
+        <v>55712.53624805016</v>
       </c>
       <c r="D25" t="n">
-        <v>66694.5444679931</v>
+        <v>67888.70682097427</v>
       </c>
       <c r="E25" t="n">
-        <v>67636.99077038727</v>
+        <v>68848.02757543912</v>
       </c>
       <c r="F25" t="n">
-        <v>60865.90290017629</v>
+        <v>61955.70372876537</v>
       </c>
       <c r="G25" t="n">
-        <v>47901.19254715493</v>
+        <v>48758.8609105718</v>
       </c>
       <c r="H25" t="n">
-        <v>34799.23307258524</v>
+        <v>35422.31153244086</v>
       </c>
     </row>
     <row r="26">
@@ -1110,25 +1110,25 @@
         <v>39448</v>
       </c>
       <c r="B26" t="n">
-        <v>32844.12415841538</v>
+        <v>33432.19649475824</v>
       </c>
       <c r="C26" t="n">
-        <v>54141.73656925637</v>
+        <v>55111.14154910522</v>
       </c>
       <c r="D26" t="n">
-        <v>65958.35531923108</v>
+        <v>67139.33624375903</v>
       </c>
       <c r="E26" t="n">
-        <v>67165.80957527905</v>
+        <v>68368.40990551708</v>
       </c>
       <c r="F26" t="n">
-        <v>60464.55026806711</v>
+        <v>61547.16489863408</v>
       </c>
       <c r="G26" t="n">
-        <v>47964.09734028512</v>
+        <v>48822.8920107542</v>
       </c>
       <c r="H26" t="n">
-        <v>35235.37276692196</v>
+        <v>35866.26028534104</v>
       </c>
     </row>
     <row r="27">
@@ -1136,25 +1136,25 @@
         <v>39814</v>
       </c>
       <c r="B27" t="n">
-        <v>32519.98853217614</v>
+        <v>33102.25723697452</v>
       </c>
       <c r="C27" t="n">
-        <v>53411.7619058373</v>
+        <v>54368.09672727017</v>
       </c>
       <c r="D27" t="n">
-        <v>64853.12539185755</v>
+        <v>66014.31723196797</v>
       </c>
       <c r="E27" t="n">
-        <v>66359.71920343945</v>
+        <v>67547.88652745754</v>
       </c>
       <c r="F27" t="n">
-        <v>59724.06271398777</v>
+        <v>60793.41895337757</v>
       </c>
       <c r="G27" t="n">
-        <v>47990.74526439238</v>
+        <v>48850.01706455777</v>
       </c>
       <c r="H27" t="n">
-        <v>35489.77009795756</v>
+        <v>36125.21258736932</v>
       </c>
     </row>
     <row r="28">
@@ -1162,25 +1162,25 @@
         <v>40179</v>
       </c>
       <c r="B28" t="n">
-        <v>32339.03953678458</v>
+        <v>32918.06835922332</v>
       </c>
       <c r="C28" t="n">
-        <v>52792.00024417508</v>
+        <v>53737.2382652613</v>
       </c>
       <c r="D28" t="n">
-        <v>63792.88432709996</v>
+        <v>64935.09260604021</v>
       </c>
       <c r="E28" t="n">
-        <v>65625.37846932012</v>
+        <v>66800.39746065324</v>
       </c>
       <c r="F28" t="n">
-        <v>59055.76289226034</v>
+        <v>60113.15325806957</v>
       </c>
       <c r="G28" t="n">
-        <v>48099.46596636599</v>
+        <v>48960.68440505057</v>
       </c>
       <c r="H28" t="n">
-        <v>35671.99779578111</v>
+        <v>36310.70306265304</v>
       </c>
     </row>
     <row r="29">
@@ -1188,25 +1188,25 @@
         <v>40544</v>
       </c>
       <c r="B29" t="n">
-        <v>32424.01994679198</v>
+        <v>33004.57033905597</v>
       </c>
       <c r="C29" t="n">
-        <v>52377.02020313522</v>
+        <v>53314.82802815066</v>
       </c>
       <c r="D29" t="n">
-        <v>63144.36230668227</v>
+        <v>64274.95883254676</v>
       </c>
       <c r="E29" t="n">
-        <v>65343.25205628965</v>
+        <v>66513.21958885776</v>
       </c>
       <c r="F29" t="n">
-        <v>58778.70920553605</v>
+        <v>59831.13893948132</v>
       </c>
       <c r="G29" t="n">
-        <v>48493.12621697097</v>
+        <v>49361.39312198662</v>
       </c>
       <c r="H29" t="n">
-        <v>35940.31572085478</v>
+        <v>36583.82520623227</v>
       </c>
     </row>
     <row r="30">
@@ -1214,25 +1214,25 @@
         <v>40909</v>
       </c>
       <c r="B30" t="n">
-        <v>32624.84124686646</v>
+        <v>33208.98733407279</v>
       </c>
       <c r="C30" t="n">
-        <v>52135.31230705106</v>
+        <v>53068.79236474723</v>
       </c>
       <c r="D30" t="n">
-        <v>63044.05107302976</v>
+        <v>64172.85153146828</v>
       </c>
       <c r="E30" t="n">
-        <v>65706.81247436465</v>
+        <v>66883.28953732633</v>
       </c>
       <c r="F30" t="n">
-        <v>58841.23827743941</v>
+        <v>59894.78759116784</v>
       </c>
       <c r="G30" t="n">
-        <v>49071.96720579739</v>
+        <v>49950.59822863914</v>
       </c>
       <c r="H30" t="n">
-        <v>36376.75695604014</v>
+        <v>37028.08089905431</v>
       </c>
     </row>
     <row r="31">
@@ -1240,25 +1240,25 @@
         <v>41275</v>
       </c>
       <c r="B31" t="n">
-        <v>32834.78650459518</v>
+        <v>33422.6916507316</v>
       </c>
       <c r="C31" t="n">
-        <v>52069.35131908502</v>
+        <v>53001.65034871917</v>
       </c>
       <c r="D31" t="n">
-        <v>63552.12670721896</v>
+        <v>64690.02423348597</v>
       </c>
       <c r="E31" t="n">
-        <v>66616.70758293728</v>
+        <v>67809.476270536</v>
       </c>
       <c r="F31" t="n">
-        <v>59170.56204153313</v>
+        <v>60230.00788014476</v>
       </c>
       <c r="G31" t="n">
-        <v>49785.14036644632</v>
+        <v>50676.54071767023</v>
       </c>
       <c r="H31" t="n">
-        <v>37034.56259670904</v>
+        <v>37697.66451553714</v>
       </c>
     </row>
     <row r="32">
@@ -1266,25 +1266,25 @@
         <v>41640</v>
       </c>
       <c r="B32" t="n">
-        <v>33117.43057229706</v>
+        <v>33710.39644577842</v>
       </c>
       <c r="C32" t="n">
-        <v>52347.25540760829</v>
+        <v>53284.53029550634</v>
       </c>
       <c r="D32" t="n">
-        <v>64627.06665886901</v>
+        <v>65784.21092911209</v>
       </c>
       <c r="E32" t="n">
-        <v>68137.53338776821</v>
+        <v>69357.53238237416</v>
       </c>
       <c r="F32" t="n">
-        <v>59835.9711900694</v>
+        <v>60907.33114490833</v>
       </c>
       <c r="G32" t="n">
-        <v>50622.40694943574</v>
+        <v>51528.79851532031</v>
       </c>
       <c r="H32" t="n">
-        <v>37907.68802246134</v>
+        <v>38586.42320666646</v>
       </c>
     </row>
     <row r="33">
@@ -1292,25 +1292,25 @@
         <v>42005</v>
       </c>
       <c r="B33" t="n">
-        <v>33409.08738668279</v>
+        <v>34007.27536027006</v>
       </c>
       <c r="C33" t="n">
-        <v>52926.4787430517</v>
+        <v>53874.12459467207</v>
       </c>
       <c r="D33" t="n">
-        <v>65982.94378644614</v>
+        <v>67164.36496620174</v>
       </c>
       <c r="E33" t="n">
-        <v>69880.26379765406</v>
+        <v>71131.46628968956</v>
       </c>
       <c r="F33" t="n">
-        <v>60882.62080095406</v>
+        <v>61972.72096268774</v>
       </c>
       <c r="G33" t="n">
-        <v>51498.89001712958</v>
+        <v>52420.9749667956</v>
       </c>
       <c r="H33" t="n">
-        <v>38864.01374986453</v>
+        <v>39559.87189652432</v>
       </c>
     </row>
     <row r="34">
@@ -1318,25 +1318,25 @@
         <v>42370</v>
       </c>
       <c r="B34" t="n">
-        <v>33685.43091340027</v>
+        <v>34288.56680347348</v>
       </c>
       <c r="C34" t="n">
-        <v>53608.97277332742</v>
+        <v>54568.83864509473</v>
       </c>
       <c r="D34" t="n">
-        <v>67349.85980695723</v>
+        <v>68555.75554702959</v>
       </c>
       <c r="E34" t="n">
-        <v>71412.01443121604</v>
+        <v>72690.64283874938</v>
       </c>
       <c r="F34" t="n">
-        <v>62115.42058308953</v>
+        <v>63227.59396086118</v>
       </c>
       <c r="G34" t="n">
-        <v>52336.65916157435</v>
+        <v>53273.74432423768</v>
       </c>
       <c r="H34" t="n">
-        <v>39779.86636247927</v>
+        <v>40492.12280257665</v>
       </c>
     </row>
     <row r="35">
@@ -1344,25 +1344,25 @@
         <v>42736</v>
       </c>
       <c r="B35" t="n">
-        <v>33968.68518116836</v>
+        <v>34576.89272418692</v>
       </c>
       <c r="C35" t="n">
-        <v>54281.47131411292</v>
+        <v>55253.37823730725</v>
       </c>
       <c r="D35" t="n">
-        <v>68625.90398591002</v>
+        <v>69854.6472306981</v>
       </c>
       <c r="E35" t="n">
-        <v>72557.82324174588</v>
+        <v>73856.9672964909</v>
       </c>
       <c r="F35" t="n">
-        <v>63245.68051915828</v>
+        <v>64378.09114235226</v>
       </c>
       <c r="G35" t="n">
-        <v>52943.85990080411</v>
+        <v>53891.81696115074</v>
       </c>
       <c r="H35" t="n">
-        <v>40571.60333796463</v>
+        <v>41298.03578746622</v>
       </c>
     </row>
     <row r="36">
@@ -1370,25 +1370,25 @@
         <v>43101</v>
       </c>
       <c r="B36" t="n">
-        <v>34501.07330539</v>
+        <v>35118.81323010771</v>
       </c>
       <c r="C36" t="n">
-        <v>54853.73379244618</v>
+        <v>55835.88704557788</v>
       </c>
       <c r="D36" t="n">
-        <v>69748.78554427918</v>
+        <v>70997.63392502052</v>
       </c>
       <c r="E36" t="n">
-        <v>73305.1305478115</v>
+        <v>74617.6551010385</v>
       </c>
       <c r="F36" t="n">
-        <v>64018.42098973638</v>
+        <v>65164.66749090133</v>
       </c>
       <c r="G36" t="n">
-        <v>53031.91118917164</v>
+        <v>53981.44480326099</v>
       </c>
       <c r="H36" t="n">
-        <v>41084.37538581208</v>
+        <v>41819.98899218474</v>
       </c>
     </row>
     <row r="37">
@@ -1396,25 +1396,25 @@
         <v>43466</v>
       </c>
       <c r="B37" t="n">
-        <v>35486.52331659802</v>
+        <v>36121.90767255844</v>
       </c>
       <c r="C37" t="n">
-        <v>55400.69648552994</v>
+        <v>56392.64307725892</v>
       </c>
       <c r="D37" t="n">
-        <v>70720.48347888674</v>
+        <v>71986.73006065389</v>
       </c>
       <c r="E37" t="n">
-        <v>73865.38182372961</v>
+        <v>75187.93764693913</v>
       </c>
       <c r="F37" t="n">
-        <v>64448.11996619085</v>
+        <v>65602.06020520019</v>
       </c>
       <c r="G37" t="n">
-        <v>52641.15057097645</v>
+        <v>53583.68763650253</v>
       </c>
       <c r="H37" t="n">
-        <v>41365.03768249198</v>
+        <v>42105.67653270228</v>
       </c>
     </row>
     <row r="38">
@@ -1422,25 +1422,25 @@
         <v>43831</v>
       </c>
       <c r="B38" t="n">
-        <v>36594.21573727777</v>
+        <v>37249.43326847029</v>
       </c>
       <c r="C38" t="n">
-        <v>56055.80031444156</v>
+        <v>57059.47650618546</v>
       </c>
       <c r="D38" t="n">
-        <v>71520.67354245477</v>
+        <v>72801.24748572899</v>
       </c>
       <c r="E38" t="n">
-        <v>74523.83624095318</v>
+        <v>75858.18165628714</v>
       </c>
       <c r="F38" t="n">
-        <v>64669.93204009067</v>
+        <v>65827.84381275695</v>
       </c>
       <c r="G38" t="n">
-        <v>52128.60580531023</v>
+        <v>53061.96578344086</v>
       </c>
       <c r="H38" t="n">
-        <v>41646.97878493027</v>
+        <v>42392.66577592886</v>
       </c>
     </row>
     <row r="39">
@@ -1448,25 +1448,25 @@
         <v>44197</v>
       </c>
       <c r="B39" t="n">
-        <v>37834.65012271873</v>
+        <v>38512.07756712458</v>
       </c>
       <c r="C39" t="n">
-        <v>56883.4796182192</v>
+        <v>57901.97536488777</v>
       </c>
       <c r="D39" t="n">
-        <v>72340.72461026347</v>
+        <v>73635.98152529351</v>
       </c>
       <c r="E39" t="n">
-        <v>75663.34844163271</v>
+        <v>77018.0967637063</v>
       </c>
       <c r="F39" t="n">
-        <v>65202.41629773637</v>
+        <v>66369.86217336563</v>
       </c>
       <c r="G39" t="n">
-        <v>51895.56122992972</v>
+        <v>52824.74855704819</v>
       </c>
       <c r="H39" t="n">
-        <v>42266.84973149897</v>
+        <v>43023.63547958494</v>
       </c>
     </row>
     <row r="40">
@@ -1474,25 +1474,25 @@
         <v>44562</v>
       </c>
       <c r="B40" t="n">
-        <v>39140.15050511227</v>
+        <v>39840.95286602573</v>
       </c>
       <c r="C40" t="n">
-        <v>57726.87047835592</v>
+        <v>58760.46709454913</v>
       </c>
       <c r="D40" t="n">
-        <v>73192.36531232699</v>
+        <v>74502.87080987265</v>
       </c>
       <c r="E40" t="n">
-        <v>77092.07875497495</v>
+        <v>78472.40841906633</v>
       </c>
       <c r="F40" t="n">
-        <v>66069.81503459088</v>
+        <v>67252.7916395301</v>
       </c>
       <c r="G40" t="n">
-        <v>51940.02411061198</v>
+        <v>52870.0075432985</v>
       </c>
       <c r="H40" t="n">
-        <v>43083.63027318</v>
+        <v>43855.04043442155</v>
       </c>
     </row>
     <row r="41">
@@ -1500,25 +1500,25 @@
         <v>44927</v>
       </c>
       <c r="B41" t="n">
-        <v>40491.08483506885</v>
+        <v>41216.07560496016</v>
       </c>
       <c r="C41" t="n">
-        <v>58601.62984635219</v>
+        <v>59650.88898357334</v>
       </c>
       <c r="D41" t="n">
-        <v>74088.27317623403</v>
+        <v>75414.81985752781</v>
       </c>
       <c r="E41" t="n">
-        <v>78680.55927066926</v>
+        <v>80089.33059585026</v>
       </c>
       <c r="F41" t="n">
-        <v>67109.86868250769</v>
+        <v>68311.46739396745</v>
       </c>
       <c r="G41" t="n">
-        <v>52154.65526828061</v>
+        <v>53088.48166069209</v>
       </c>
       <c r="H41" t="n">
-        <v>43834.80415495108</v>
+        <v>44619.66404551171</v>
       </c>
     </row>
   </sheetData>

</xml_diff>